<commit_message>
Updates 16S reference BD with rename to specify date; Uploads reference documentation (Word file)
</commit_message>
<xml_diff>
--- a/DADA2/WADE003-arcticpred-16SP2-taxa.xlsx
+++ b/DADA2/WADE003-arcticpred-16SP2-taxa.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic Predator Diets/DADA2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/DADA2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_1FE63DD28F79A8D366075C52F37BD2728A4576ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C2CE2D8-AE2A-4EE6-8698-1F8BBFD61BC5}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="11_1FE63DD28F79A8D366075C52F37BD2728A4576ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{453BF1E7-3937-4952-BD72-FE2C40923610}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -374,9 +373,6 @@
     <t>Myoxocephalus sp; ASK AMY</t>
   </si>
   <si>
-    <t>closely related pike species; ASK AMY</t>
-  </si>
-  <si>
     <t>Salvelinus sp.; ASK AMY</t>
   </si>
   <si>
@@ -393,13 +389,16 @@
   </si>
   <si>
     <t>bacteria sp.</t>
+  </si>
+  <si>
+    <t>Esox sp. ; closely related pike species; ASK AMY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,8 +414,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +435,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -439,17 +450,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -758,13 +772,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="87" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -797,37 +815,37 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>110</v>
       </c>
     </row>
@@ -874,20 +892,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>109</v>
       </c>
     </row>
@@ -960,29 +978,29 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1187,37 +1205,37 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1351,12 +1369,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I30" t="s">
-        <v>117</v>
+      <c r="I30" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1427,7 +1445,7 @@
         <v>16</v>
       </c>
       <c r="I34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1549,7 +1567,7 @@
         <v>89</v>
       </c>
       <c r="I41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1680,52 +1698,52 @@
         <v>111</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" t="s">
+      <c r="B52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I52" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I54" s="3" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>101</v>
-      </c>
-      <c r="I53" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>102</v>
-      </c>
-      <c r="B54" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" t="s">
-        <v>74</v>
-      </c>
-      <c r="E54" t="s">
-        <v>75</v>
-      </c>
-      <c r="I54" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -1759,7 +1777,7 @@
         <v>104</v>
       </c>
       <c r="I56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates 12S and 16S reference databases with >99% matches (both for species and genus); Updates 16S from Pleuronectiformes to Carangiformes; Fixes incorrect mapping of ADFG IDs to plots for 16S and 12S; Saves new outputs from DADA2 pipelines after updates to reference databases.
</commit_message>
<xml_diff>
--- a/DADA2/WADE003-arcticpred-16SP2-taxa.xlsx
+++ b/DADA2/WADE003-arcticpred-16SP2-taxa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/DADA2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\DADA2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="11_1FE63DD28F79A8D366075C52F37BD2728A4576ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA53473A-A85E-4252-8AF5-C6B9C2F498C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A458D0-8F14-47AE-BC1D-B3602E753B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3270" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="142">
   <si>
     <t>rownames</t>
   </si>
@@ -376,72 +376,39 @@
     <t>Esox sp. ; closely related pike species; ASK AMY</t>
   </si>
   <si>
-    <t>no 100% match: 99.73% Myoxocephalus aenaeus, Myoxocephalus scorpius</t>
-  </si>
-  <si>
     <t>Myzopsetta proboscidea</t>
   </si>
   <si>
     <t>100% matches: Liopsetta pinnifasciata, Liopsetta glacialis</t>
   </si>
   <si>
-    <t>100% matches: Pleuronectes quadrituberculatus, Parophrys vetulus, Psettichthys melanostictus</t>
-  </si>
-  <si>
-    <t>100% matches: Lumpenus fabricii, Leptoclinus maculatus</t>
-  </si>
-  <si>
     <t>no 100% match: 99.73% Gymnocanthus pistilliger, Gymnocanthus intermedius</t>
   </si>
   <si>
     <t>no 100% match: 99.73% Gymnocanthus tricuspis</t>
   </si>
   <si>
-    <t>no 100% matches: Pusa and Phoca sp. - MAMMALIA</t>
-  </si>
-  <si>
-    <t>no 100% match: 99.73% Microcottus sellaris, Myoxocephalus verrucosus, Myoxocephalus scorpius</t>
-  </si>
-  <si>
     <t>100% matches: Lumpenus fabricii, Lumpenus lampretaeformis</t>
   </si>
   <si>
     <t>no 100% matches: 99.07% Erignathus barbatus</t>
   </si>
   <si>
-    <t>no 100% match: 99.73% Myoxocephalus jaok</t>
-  </si>
-  <si>
     <t xml:space="preserve">100% matches: Myoxocephalus quadricornis, Myoxocephalus aenaeus, Myoxocephalus thompsonii, Myoxocephalus scorpius, </t>
   </si>
   <si>
     <t>no 100% matches: 98.57% Delphinapterus leucas</t>
   </si>
   <si>
-    <t>100% matches: Salvelinus malma, Salvelinus curilus, Salvethymus svetovidovi, Salvelinus alpinus, Salvelinus elgyticus, Salvelinus kuznetzovi, Salvelinus kronocius, Salvelinus schmidti, Salvelinus albus</t>
-  </si>
-  <si>
-    <t>no 100% match: 99.07% Pusa hispida, Phoca siberica</t>
-  </si>
-  <si>
-    <t>no 100% match: 99.54% Gymnocanthus tricuspis</t>
-  </si>
-  <si>
     <t>100% matches: Limanda limanda, Limanda aspera</t>
   </si>
   <si>
-    <t>100% matches: Leptoclinus maculatus, Lumpenus fabricii</t>
-  </si>
-  <si>
     <t>no 100% match: 99.07% Erignathus barbatus</t>
   </si>
   <si>
     <t>no 100% match: 97.17% Pusa hispida</t>
   </si>
   <si>
-    <t>no 100% match: Podothecus sachi, Leptagonus decagonus, Podothecus accipenserinus, Sarritor frenatus</t>
-  </si>
-  <si>
     <t>no 100% match: 91.49% Gadus macrocephalus</t>
   </si>
   <si>
@@ -449,13 +416,43 @@
   </si>
   <si>
     <t>no 100% match: 98.97% Helicobacter sp.</t>
+  </si>
+  <si>
+    <t>100% matches: Salvelinus malma, Salvelinus curilus, Salvelinus alpinus, Salvelinus elgyticus, Salvelinus kuznetzovi, Salvelinus kronocius, Salvelinus schmidti, Salvelinus albus</t>
+  </si>
+  <si>
+    <t>no 100% matches: &gt;98% Pusa hispida, Pusa vitulina</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.54% Gymnocanthus tricuspis, &gt;98% Gymnocanthus spp., Triglops scepticus</t>
+  </si>
+  <si>
+    <t>100% matches: Lumpenus fabricii, Leptoclinus maculatus; Stichaeidae</t>
+  </si>
+  <si>
+    <t>100% matches: Pleuronectes quadrituberculatus, Parophrys vetulus, Psettichthys melanostictus; Pleuronectidae</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.73% Myoxocephalus aenaeus, Myoxocephalus scorpius; &gt;98% Myoxocephalus spp., Microcottus sellaris, Porocottus minutus; Cottidae</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.73% Microcottus sellaris, Myoxocephalus verrucosus, Myoxocephalus scorpius; Psychrolutidae</t>
+  </si>
+  <si>
+    <t>no 100% match: 99.73% Myoxocephalus jaok; &gt;98% Myococephalus spp., Microcottus stellaris; Psychrolutidae</t>
+  </si>
+  <si>
+    <t>100% matches: Leptoclinus maculatus, Lumpenus fabricii; Stichaeidae</t>
+  </si>
+  <si>
+    <t>no 100% match: Podothecus sachi, Leptagonus decagonus, Podothecus accipenserinus, Sarritor frenatus; Agonidae</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -478,8 +475,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -489,6 +493,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -501,19 +510,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,10 +539,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -822,21 +830,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:XFD56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="67.28515625" customWidth="1"/>
+    <col min="1" max="1" width="40" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.265625" customWidth="1"/>
+    <col min="6" max="6" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -865,7 +873,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -882,7 +890,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -899,7 +907,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -913,10 +921,10 @@
         <v>11</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -942,7 +950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -959,7 +967,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -985,7 +993,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1011,24 +1019,24 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -1054,7 +1062,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1080,38 +1088,38 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1137,7 +1145,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1163,27 +1171,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I16" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I16" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1209,27 +1217,27 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1255,7 +1263,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
@@ -1275,7 +1283,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
@@ -1289,35 +1297,35 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
-      </c>
-      <c r="I22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1343,35 +1351,35 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I25" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="I25" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B26" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="B26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I26" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -1397,29 +1405,29 @@
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
-      </c>
-      <c r="I28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>70</v>
       </c>
@@ -1427,98 +1435,98 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="B31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="I31" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="I32" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="B33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I33" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="I33" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="B34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B35" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="B35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I35" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -1544,7 +1552,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -1570,15 +1578,15 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -1604,7 +1612,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -1612,31 +1620,31 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I41" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="I41" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="I43" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>92</v>
       </c>
@@ -1662,59 +1670,59 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A45" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I45" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="I45" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B46" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" t="s">
-        <v>10</v>
-      </c>
-      <c r="I46" t="s">
+      <c r="B46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>95</v>
-      </c>
-      <c r="B47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" t="s">
-        <v>10</v>
-      </c>
-      <c r="I47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>96</v>
-      </c>
-      <c r="I48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>97</v>
-      </c>
-      <c r="I49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -1740,15 +1748,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I51" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I51" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>100</v>
       </c>
@@ -1768,7 +1776,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A53" s="2" t="s">
         <v>101</v>
       </c>
@@ -1776,7 +1784,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A54" s="2" t="s">
         <v>102</v>
       </c>
@@ -1796,7 +1804,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>103</v>
       </c>
@@ -1822,15 +1830,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I56" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>105</v>
       </c>
@@ -1838,30 +1846,30 @@
         <v>9</v>
       </c>
       <c r="I57" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="B58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I58" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I58" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>107</v>
       </c>

</xml_diff>